<commit_message>
Atualizado por script em 12-11-2023 08:45
</commit_message>
<xml_diff>
--- a/2023/colombia_primera-b_2023.xlsx
+++ b/2023/colombia_primera-b_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V129"/>
+  <dimension ref="A1:V153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2045,22 +2045,22 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Orsomarso</t>
+          <t>Real Santander</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Fortaleza</t>
+          <t>Patriotas</t>
         </is>
       </c>
       <c r="I18" t="n">
         <v>1</v>
       </c>
       <c r="J18" t="n">
-        <v>4.34</v>
+        <v>2.63</v>
       </c>
       <c r="K18" t="inlineStr">
         <is>
@@ -2068,15 +2068,15 @@
         </is>
       </c>
       <c r="L18" t="n">
-        <v>4.26</v>
+        <v>2.97</v>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>05/08/2023 17:21</t>
+          <t>05/08/2023 22:21</t>
         </is>
       </c>
       <c r="N18" t="n">
-        <v>3.3</v>
+        <v>2.91</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -2084,15 +2084,15 @@
         </is>
       </c>
       <c r="P18" t="n">
-        <v>3.21</v>
+        <v>2.81</v>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>05/08/2023 17:21</t>
+          <t>05/08/2023 22:29</t>
         </is>
       </c>
       <c r="R18" t="n">
-        <v>1.85</v>
+        <v>3.13</v>
       </c>
       <c r="S18" t="inlineStr">
         <is>
@@ -2100,16 +2100,16 @@
         </is>
       </c>
       <c r="T18" t="n">
-        <v>2</v>
+        <v>2.85</v>
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>05/08/2023 17:21</t>
+          <t>05/08/2023 22:21</t>
         </is>
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/colombia/primera-b/orsomarso-fortaleza-c-e-i-f/zZ6aqAE3/</t>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/real-santander-patriotas/Q3P8Mn7j/</t>
         </is>
       </c>
     </row>
@@ -2137,22 +2137,22 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Real Santander</t>
+          <t>Orsomarso</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Patriotas</t>
+          <t>Fortaleza</t>
         </is>
       </c>
       <c r="I19" t="n">
         <v>1</v>
       </c>
       <c r="J19" t="n">
-        <v>2.63</v>
+        <v>4.34</v>
       </c>
       <c r="K19" t="inlineStr">
         <is>
@@ -2160,15 +2160,15 @@
         </is>
       </c>
       <c r="L19" t="n">
-        <v>2.97</v>
+        <v>4.26</v>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>05/08/2023 22:21</t>
+          <t>05/08/2023 17:21</t>
         </is>
       </c>
       <c r="N19" t="n">
-        <v>2.91</v>
+        <v>3.3</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
@@ -2176,15 +2176,15 @@
         </is>
       </c>
       <c r="P19" t="n">
-        <v>2.81</v>
+        <v>3.21</v>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>05/08/2023 22:29</t>
+          <t>05/08/2023 17:21</t>
         </is>
       </c>
       <c r="R19" t="n">
-        <v>3.13</v>
+        <v>1.85</v>
       </c>
       <c r="S19" t="inlineStr">
         <is>
@@ -2192,16 +2192,16 @@
         </is>
       </c>
       <c r="T19" t="n">
-        <v>2.85</v>
+        <v>2</v>
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>05/08/2023 22:21</t>
+          <t>05/08/2023 17:21</t>
         </is>
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/colombia/primera-b/real-santander-patriotas/Q3P8Mn7j/</t>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/orsomarso-fortaleza-c-e-i-f/zZ6aqAE3/</t>
         </is>
       </c>
     </row>
@@ -2873,7 +2873,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Cucuta</t>
+          <t>Leones</t>
         </is>
       </c>
       <c r="G27" t="n">
@@ -2881,63 +2881,63 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Barranquilla</t>
+          <t>Atletico F.C.</t>
         </is>
       </c>
       <c r="I27" t="n">
         <v>2</v>
       </c>
       <c r="J27" t="n">
-        <v>1.4</v>
+        <v>1.76</v>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>09/08/2023 03:12</t>
+          <t>07/08/2023 22:12</t>
         </is>
       </c>
       <c r="L27" t="n">
-        <v>1.4</v>
+        <v>1.67</v>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>12/08/2023 22:28</t>
+          <t>12/08/2023 22:21</t>
         </is>
       </c>
       <c r="N27" t="n">
-        <v>4.44</v>
+        <v>3.59</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>09/08/2023 03:12</t>
+          <t>07/08/2023 22:12</t>
         </is>
       </c>
       <c r="P27" t="n">
-        <v>4.71</v>
+        <v>3.73</v>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>12/08/2023 22:28</t>
+          <t>12/08/2023 22:24</t>
         </is>
       </c>
       <c r="R27" t="n">
-        <v>6.99</v>
+        <v>4.75</v>
       </c>
       <c r="S27" t="inlineStr">
         <is>
-          <t>09/08/2023 03:12</t>
+          <t>07/08/2023 22:12</t>
         </is>
       </c>
       <c r="T27" t="n">
-        <v>8.119999999999999</v>
+        <v>5.47</v>
       </c>
       <c r="U27" t="inlineStr">
         <is>
-          <t>12/08/2023 22:28</t>
+          <t>12/08/2023 22:21</t>
         </is>
       </c>
       <c r="V27" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/colombia/primera-b/cucuta-barranquilla/UeSYc9Td/</t>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/leones-atletico-f-c/KQprynMq/</t>
         </is>
       </c>
     </row>
@@ -2965,7 +2965,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Leones</t>
+          <t>Cucuta</t>
         </is>
       </c>
       <c r="G28" t="n">
@@ -2973,63 +2973,63 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Atletico F.C.</t>
+          <t>Barranquilla</t>
         </is>
       </c>
       <c r="I28" t="n">
         <v>2</v>
       </c>
       <c r="J28" t="n">
-        <v>1.76</v>
+        <v>1.4</v>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>07/08/2023 22:12</t>
+          <t>09/08/2023 03:12</t>
         </is>
       </c>
       <c r="L28" t="n">
-        <v>1.67</v>
+        <v>1.4</v>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>12/08/2023 22:21</t>
+          <t>12/08/2023 22:28</t>
         </is>
       </c>
       <c r="N28" t="n">
-        <v>3.59</v>
+        <v>4.44</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>07/08/2023 22:12</t>
+          <t>09/08/2023 03:12</t>
         </is>
       </c>
       <c r="P28" t="n">
-        <v>3.73</v>
+        <v>4.71</v>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>12/08/2023 22:24</t>
+          <t>12/08/2023 22:28</t>
         </is>
       </c>
       <c r="R28" t="n">
-        <v>4.75</v>
+        <v>6.99</v>
       </c>
       <c r="S28" t="inlineStr">
         <is>
-          <t>07/08/2023 22:12</t>
+          <t>09/08/2023 03:12</t>
         </is>
       </c>
       <c r="T28" t="n">
-        <v>5.47</v>
+        <v>8.119999999999999</v>
       </c>
       <c r="U28" t="inlineStr">
         <is>
-          <t>12/08/2023 22:21</t>
+          <t>12/08/2023 22:28</t>
         </is>
       </c>
       <c r="V28" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/colombia/primera-b/leones-atletico-f-c/KQprynMq/</t>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/cucuta-barranquilla/UeSYc9Td/</t>
         </is>
       </c>
     </row>
@@ -4437,34 +4437,34 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Real Soacha</t>
+          <t>Boca Juniors</t>
         </is>
       </c>
       <c r="G44" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Tigres</t>
+          <t>Patriotas</t>
         </is>
       </c>
       <c r="I44" t="n">
         <v>0</v>
       </c>
       <c r="J44" t="n">
-        <v>1.99</v>
+        <v>3.9</v>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>23/08/2023 21:27</t>
+          <t>20/08/2023 22:42</t>
         </is>
       </c>
       <c r="L44" t="n">
-        <v>2.75</v>
+        <v>2.58</v>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>24/08/2023 22:10</t>
+          <t>24/08/2023 22:29</t>
         </is>
       </c>
       <c r="N44" t="n">
@@ -4472,36 +4472,36 @@
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>23/08/2023 21:27</t>
+          <t>20/08/2023 22:42</t>
         </is>
       </c>
       <c r="P44" t="n">
-        <v>2.9</v>
+        <v>3.09</v>
       </c>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>24/08/2023 19:45</t>
+          <t>24/08/2023 22:29</t>
         </is>
       </c>
       <c r="R44" t="n">
-        <v>4.03</v>
+        <v>2.1</v>
       </c>
       <c r="S44" t="inlineStr">
         <is>
-          <t>23/08/2023 21:27</t>
+          <t>20/08/2023 22:42</t>
         </is>
       </c>
       <c r="T44" t="n">
-        <v>2.98</v>
+        <v>3.01</v>
       </c>
       <c r="U44" t="inlineStr">
         <is>
-          <t>24/08/2023 22:10</t>
+          <t>24/08/2023 22:29</t>
         </is>
       </c>
       <c r="V44" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/colombia/primera-b/real-soacha-tigres-futbol-club/ltg8btK7/</t>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/boca-juniors-de-cali-patriotas/IiFP64CR/</t>
         </is>
       </c>
     </row>
@@ -4529,34 +4529,34 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Boca Juniors</t>
+          <t>Real Soacha</t>
         </is>
       </c>
       <c r="G45" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Patriotas</t>
+          <t>Tigres</t>
         </is>
       </c>
       <c r="I45" t="n">
         <v>0</v>
       </c>
       <c r="J45" t="n">
-        <v>3.9</v>
+        <v>1.99</v>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>20/08/2023 22:42</t>
+          <t>23/08/2023 21:27</t>
         </is>
       </c>
       <c r="L45" t="n">
-        <v>2.58</v>
+        <v>2.75</v>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>24/08/2023 22:29</t>
+          <t>24/08/2023 22:10</t>
         </is>
       </c>
       <c r="N45" t="n">
@@ -4564,36 +4564,36 @@
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>20/08/2023 22:42</t>
+          <t>23/08/2023 21:27</t>
         </is>
       </c>
       <c r="P45" t="n">
-        <v>3.09</v>
+        <v>2.9</v>
       </c>
       <c r="Q45" t="inlineStr">
         <is>
-          <t>24/08/2023 22:29</t>
+          <t>24/08/2023 19:45</t>
         </is>
       </c>
       <c r="R45" t="n">
-        <v>2.1</v>
+        <v>4.03</v>
       </c>
       <c r="S45" t="inlineStr">
         <is>
-          <t>20/08/2023 22:42</t>
+          <t>23/08/2023 21:27</t>
         </is>
       </c>
       <c r="T45" t="n">
-        <v>3.01</v>
+        <v>2.98</v>
       </c>
       <c r="U45" t="inlineStr">
         <is>
-          <t>24/08/2023 22:29</t>
+          <t>24/08/2023 22:10</t>
         </is>
       </c>
       <c r="V45" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/colombia/primera-b/boca-juniors-de-cali-patriotas/IiFP64CR/</t>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/real-soacha-tigres-futbol-club/ltg8btK7/</t>
         </is>
       </c>
     </row>
@@ -5081,71 +5081,71 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Atletico F.C.</t>
+          <t>Tigres</t>
         </is>
       </c>
       <c r="G51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Llaneros</t>
+        </is>
+      </c>
+      <c r="I51" t="n">
         <v>1</v>
       </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>Real Soacha</t>
-        </is>
-      </c>
-      <c r="I51" t="n">
-        <v>2</v>
-      </c>
       <c r="J51" t="n">
-        <v>2.27</v>
+        <v>2.55</v>
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>27/08/2023 10:42</t>
+          <t>25/08/2023 21:13</t>
         </is>
       </c>
       <c r="L51" t="n">
-        <v>2.54</v>
+        <v>2.68</v>
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>28/08/2023 21:54</t>
+          <t>28/08/2023 21:18</t>
         </is>
       </c>
       <c r="N51" t="n">
-        <v>3.06</v>
+        <v>2.9</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>27/08/2023 10:42</t>
+          <t>25/08/2023 21:13</t>
         </is>
       </c>
       <c r="P51" t="n">
-        <v>3.01</v>
+        <v>2.97</v>
       </c>
       <c r="Q51" t="inlineStr">
         <is>
-          <t>28/08/2023 21:54</t>
+          <t>28/08/2023 21:18</t>
         </is>
       </c>
       <c r="R51" t="n">
-        <v>3.47</v>
+        <v>3</v>
       </c>
       <c r="S51" t="inlineStr">
         <is>
-          <t>27/08/2023 10:42</t>
+          <t>25/08/2023 21:13</t>
         </is>
       </c>
       <c r="T51" t="n">
-        <v>3.15</v>
+        <v>3</v>
       </c>
       <c r="U51" t="inlineStr">
         <is>
-          <t>28/08/2023 21:59</t>
+          <t>28/08/2023 21:18</t>
         </is>
       </c>
       <c r="V51" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/colombia/primera-b/atletico-f-c-real-soacha/GnofMqCE/</t>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/tigres-futbol-club-llaneros/Aov3KNtR/</t>
         </is>
       </c>
     </row>
@@ -5173,71 +5173,71 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Tigres</t>
+          <t>Atletico F.C.</t>
         </is>
       </c>
       <c r="G52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Llaneros</t>
+          <t>Real Soacha</t>
         </is>
       </c>
       <c r="I52" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J52" t="n">
-        <v>2.55</v>
+        <v>2.27</v>
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>25/08/2023 21:13</t>
+          <t>27/08/2023 10:42</t>
         </is>
       </c>
       <c r="L52" t="n">
-        <v>2.68</v>
+        <v>2.54</v>
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>28/08/2023 21:18</t>
+          <t>28/08/2023 21:54</t>
         </is>
       </c>
       <c r="N52" t="n">
-        <v>2.9</v>
+        <v>3.06</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>25/08/2023 21:13</t>
+          <t>27/08/2023 10:42</t>
         </is>
       </c>
       <c r="P52" t="n">
-        <v>2.97</v>
+        <v>3.01</v>
       </c>
       <c r="Q52" t="inlineStr">
         <is>
-          <t>28/08/2023 21:18</t>
+          <t>28/08/2023 21:54</t>
         </is>
       </c>
       <c r="R52" t="n">
-        <v>3</v>
+        <v>3.47</v>
       </c>
       <c r="S52" t="inlineStr">
         <is>
-          <t>25/08/2023 21:13</t>
+          <t>27/08/2023 10:42</t>
         </is>
       </c>
       <c r="T52" t="n">
-        <v>3</v>
+        <v>3.15</v>
       </c>
       <c r="U52" t="inlineStr">
         <is>
-          <t>28/08/2023 21:18</t>
+          <t>28/08/2023 21:59</t>
         </is>
       </c>
       <c r="V52" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/colombia/primera-b/tigres-futbol-club-llaneros/Aov3KNtR/</t>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/atletico-f-c-real-soacha/GnofMqCE/</t>
         </is>
       </c>
     </row>
@@ -6001,7 +6001,7 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Cartagena</t>
+          <t>Leones</t>
         </is>
       </c>
       <c r="G61" t="n">
@@ -6009,22 +6009,22 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Orsomarso</t>
+          <t>Tigres</t>
         </is>
       </c>
       <c r="I61" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J61" t="n">
-        <v>1.64</v>
+        <v>2</v>
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>27/08/2023 23:12</t>
+          <t>30/08/2023 22:12</t>
         </is>
       </c>
       <c r="L61" t="n">
-        <v>1.56</v>
+        <v>1.83</v>
       </c>
       <c r="M61" t="inlineStr">
         <is>
@@ -6032,40 +6032,40 @@
         </is>
       </c>
       <c r="N61" t="n">
-        <v>3.79</v>
+        <v>3.26</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>27/08/2023 23:12</t>
+          <t>30/08/2023 22:12</t>
         </is>
       </c>
       <c r="P61" t="n">
+        <v>3.54</v>
+      </c>
+      <c r="Q61" t="inlineStr">
+        <is>
+          <t>03/09/2023 22:52</t>
+        </is>
+      </c>
+      <c r="R61" t="n">
         <v>4.02</v>
       </c>
-      <c r="Q61" t="inlineStr">
-        <is>
-          <t>03/09/2023 22:59</t>
-        </is>
-      </c>
-      <c r="R61" t="n">
-        <v>5.41</v>
-      </c>
       <c r="S61" t="inlineStr">
         <is>
-          <t>27/08/2023 23:12</t>
+          <t>30/08/2023 22:12</t>
         </is>
       </c>
       <c r="T61" t="n">
-        <v>6.3</v>
+        <v>4.59</v>
       </c>
       <c r="U61" t="inlineStr">
         <is>
-          <t>03/09/2023 22:59</t>
+          <t>03/09/2023 22:52</t>
         </is>
       </c>
       <c r="V61" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/colombia/primera-b/cartagena-orsomarso/QqFMDCPB/</t>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/leones-tigres-futbol-club/WMFIEhA5/</t>
         </is>
       </c>
     </row>
@@ -6093,7 +6093,7 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Leones</t>
+          <t>Cartagena</t>
         </is>
       </c>
       <c r="G62" t="n">
@@ -6101,22 +6101,22 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Tigres</t>
+          <t>Orsomarso</t>
         </is>
       </c>
       <c r="I62" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J62" t="n">
-        <v>2</v>
+        <v>1.64</v>
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>30/08/2023 22:12</t>
+          <t>27/08/2023 23:12</t>
         </is>
       </c>
       <c r="L62" t="n">
-        <v>1.83</v>
+        <v>1.56</v>
       </c>
       <c r="M62" t="inlineStr">
         <is>
@@ -6124,40 +6124,40 @@
         </is>
       </c>
       <c r="N62" t="n">
-        <v>3.26</v>
+        <v>3.79</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>30/08/2023 22:12</t>
+          <t>27/08/2023 23:12</t>
         </is>
       </c>
       <c r="P62" t="n">
-        <v>3.54</v>
+        <v>4.02</v>
       </c>
       <c r="Q62" t="inlineStr">
         <is>
-          <t>03/09/2023 22:52</t>
+          <t>03/09/2023 22:59</t>
         </is>
       </c>
       <c r="R62" t="n">
-        <v>4.02</v>
+        <v>5.41</v>
       </c>
       <c r="S62" t="inlineStr">
         <is>
-          <t>30/08/2023 22:12</t>
+          <t>27/08/2023 23:12</t>
         </is>
       </c>
       <c r="T62" t="n">
-        <v>4.59</v>
+        <v>6.3</v>
       </c>
       <c r="U62" t="inlineStr">
         <is>
-          <t>03/09/2023 22:52</t>
+          <t>03/09/2023 22:59</t>
         </is>
       </c>
       <c r="V62" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/colombia/primera-b/leones-tigres-futbol-club/WMFIEhA5/</t>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/cartagena-orsomarso/QqFMDCPB/</t>
         </is>
       </c>
     </row>
@@ -7933,71 +7933,71 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Atletico F.C.</t>
+          <t>Real Soacha</t>
         </is>
       </c>
       <c r="G82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Quindio</t>
+          <t>Patriotas</t>
         </is>
       </c>
       <c r="I82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J82" t="n">
-        <v>3.04</v>
+        <v>2.55</v>
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>11/09/2023 22:12</t>
+          <t>13/09/2023 20:42</t>
         </is>
       </c>
       <c r="L82" t="n">
-        <v>2.44</v>
+        <v>3.5</v>
       </c>
       <c r="M82" t="inlineStr">
         <is>
-          <t>15/09/2023 22:29</t>
+          <t>15/09/2023 22:12</t>
         </is>
       </c>
       <c r="N82" t="n">
-        <v>3.1</v>
+        <v>2.79</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>11/09/2023 22:12</t>
+          <t>13/09/2023 20:42</t>
         </is>
       </c>
       <c r="P82" t="n">
-        <v>3.37</v>
+        <v>2.81</v>
       </c>
       <c r="Q82" t="inlineStr">
         <is>
-          <t>15/09/2023 22:29</t>
+          <t>15/09/2023 22:12</t>
         </is>
       </c>
       <c r="R82" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="S82" t="inlineStr">
+        <is>
+          <t>13/09/2023 20:42</t>
+        </is>
+      </c>
+      <c r="T82" t="n">
         <v>2.49</v>
       </c>
-      <c r="S82" t="inlineStr">
-        <is>
-          <t>11/09/2023 22:12</t>
-        </is>
-      </c>
-      <c r="T82" t="n">
-        <v>2.67</v>
-      </c>
       <c r="U82" t="inlineStr">
         <is>
-          <t>15/09/2023 22:29</t>
+          <t>15/09/2023 22:12</t>
         </is>
       </c>
       <c r="V82" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/colombia/primera-b/atletico-f-c-quindio/QJVVvkOA/</t>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/real-soacha-patriotas/retRuV84/</t>
         </is>
       </c>
     </row>
@@ -8025,71 +8025,71 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Real Soacha</t>
+          <t>Atletico F.C.</t>
         </is>
       </c>
       <c r="G83" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Patriotas</t>
+          <t>Quindio</t>
         </is>
       </c>
       <c r="I83" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J83" t="n">
-        <v>2.55</v>
+        <v>3.04</v>
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>13/09/2023 20:42</t>
+          <t>11/09/2023 22:12</t>
         </is>
       </c>
       <c r="L83" t="n">
-        <v>3.5</v>
+        <v>2.44</v>
       </c>
       <c r="M83" t="inlineStr">
         <is>
-          <t>15/09/2023 22:12</t>
+          <t>15/09/2023 22:29</t>
         </is>
       </c>
       <c r="N83" t="n">
-        <v>2.79</v>
+        <v>3.1</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>13/09/2023 20:42</t>
+          <t>11/09/2023 22:12</t>
         </is>
       </c>
       <c r="P83" t="n">
-        <v>2.81</v>
+        <v>3.37</v>
       </c>
       <c r="Q83" t="inlineStr">
         <is>
-          <t>15/09/2023 22:12</t>
+          <t>15/09/2023 22:29</t>
         </is>
       </c>
       <c r="R83" t="n">
-        <v>3.13</v>
+        <v>2.49</v>
       </c>
       <c r="S83" t="inlineStr">
         <is>
-          <t>13/09/2023 20:42</t>
+          <t>11/09/2023 22:12</t>
         </is>
       </c>
       <c r="T83" t="n">
-        <v>2.49</v>
+        <v>2.67</v>
       </c>
       <c r="U83" t="inlineStr">
         <is>
-          <t>15/09/2023 22:12</t>
+          <t>15/09/2023 22:29</t>
         </is>
       </c>
       <c r="V83" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/colombia/primera-b/real-soacha-patriotas/retRuV84/</t>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/atletico-f-c-quindio/QJVVvkOA/</t>
         </is>
       </c>
     </row>
@@ -8945,7 +8945,7 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Real Santander</t>
+          <t>Fortaleza</t>
         </is>
       </c>
       <c r="G93" t="n">
@@ -8953,63 +8953,63 @@
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>Tigres</t>
+          <t>Cartagena</t>
         </is>
       </c>
       <c r="I93" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J93" t="n">
-        <v>1.81</v>
+        <v>1.72</v>
       </c>
       <c r="K93" t="inlineStr">
         <is>
-          <t>16/09/2023 22:42</t>
+          <t>16/09/2023 23:13</t>
         </is>
       </c>
       <c r="L93" t="n">
-        <v>1.68</v>
+        <v>1.56</v>
       </c>
       <c r="M93" t="inlineStr">
         <is>
-          <t>20/09/2023 22:22</t>
+          <t>20/09/2023 22:21</t>
         </is>
       </c>
       <c r="N93" t="n">
-        <v>3.3</v>
+        <v>3.6</v>
       </c>
       <c r="O93" t="inlineStr">
         <is>
-          <t>16/09/2023 22:42</t>
+          <t>16/09/2023 23:13</t>
         </is>
       </c>
       <c r="P93" t="n">
-        <v>3.75</v>
+        <v>3.95</v>
       </c>
       <c r="Q93" t="inlineStr">
         <is>
-          <t>20/09/2023 22:22</t>
+          <t>20/09/2023 22:21</t>
         </is>
       </c>
       <c r="R93" t="n">
-        <v>4.51</v>
+        <v>4.97</v>
       </c>
       <c r="S93" t="inlineStr">
         <is>
-          <t>16/09/2023 22:42</t>
+          <t>16/09/2023 23:13</t>
         </is>
       </c>
       <c r="T93" t="n">
-        <v>5.31</v>
+        <v>6.48</v>
       </c>
       <c r="U93" t="inlineStr">
         <is>
-          <t>20/09/2023 22:22</t>
+          <t>20/09/2023 22:21</t>
         </is>
       </c>
       <c r="V93" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/colombia/primera-b/real-santander-tigres-futbol-club/ABZmoQpp/</t>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/fortaleza-c-e-i-f-cartagena/QwbHjnNM/</t>
         </is>
       </c>
     </row>
@@ -9037,7 +9037,7 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>Fortaleza</t>
+          <t>Real Santander</t>
         </is>
       </c>
       <c r="G94" t="n">
@@ -9045,63 +9045,63 @@
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>Cartagena</t>
+          <t>Tigres</t>
         </is>
       </c>
       <c r="I94" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J94" t="n">
-        <v>1.72</v>
+        <v>1.81</v>
       </c>
       <c r="K94" t="inlineStr">
         <is>
-          <t>16/09/2023 23:13</t>
+          <t>16/09/2023 22:42</t>
         </is>
       </c>
       <c r="L94" t="n">
-        <v>1.56</v>
+        <v>1.68</v>
       </c>
       <c r="M94" t="inlineStr">
         <is>
-          <t>20/09/2023 22:21</t>
+          <t>20/09/2023 22:22</t>
         </is>
       </c>
       <c r="N94" t="n">
-        <v>3.6</v>
+        <v>3.3</v>
       </c>
       <c r="O94" t="inlineStr">
         <is>
-          <t>16/09/2023 23:13</t>
+          <t>16/09/2023 22:42</t>
         </is>
       </c>
       <c r="P94" t="n">
-        <v>3.95</v>
+        <v>3.75</v>
       </c>
       <c r="Q94" t="inlineStr">
         <is>
-          <t>20/09/2023 22:21</t>
+          <t>20/09/2023 22:22</t>
         </is>
       </c>
       <c r="R94" t="n">
-        <v>4.97</v>
+        <v>4.51</v>
       </c>
       <c r="S94" t="inlineStr">
         <is>
-          <t>16/09/2023 23:13</t>
+          <t>16/09/2023 22:42</t>
         </is>
       </c>
       <c r="T94" t="n">
-        <v>6.48</v>
+        <v>5.31</v>
       </c>
       <c r="U94" t="inlineStr">
         <is>
-          <t>20/09/2023 22:21</t>
+          <t>20/09/2023 22:22</t>
         </is>
       </c>
       <c r="V94" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/colombia/primera-b/fortaleza-c-e-i-f-cartagena/QwbHjnNM/</t>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/real-santander-tigres-futbol-club/ABZmoQpp/</t>
         </is>
       </c>
     </row>
@@ -12322,6 +12322,2214 @@
       <c r="V129" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/colombia/primera-b/real-soacha-real-santander/hjqVcOom/</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>primera-b</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E130" s="2" t="n">
+        <v>45215.9375</v>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>Boca Juniors</t>
+        </is>
+      </c>
+      <c r="G130" t="n">
+        <v>1</v>
+      </c>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>Fortaleza</t>
+        </is>
+      </c>
+      <c r="I130" t="n">
+        <v>1</v>
+      </c>
+      <c r="J130" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="K130" t="inlineStr">
+        <is>
+          <t>13/10/2023 06:12</t>
+        </is>
+      </c>
+      <c r="L130" t="n">
+        <v>3.66</v>
+      </c>
+      <c r="M130" t="inlineStr">
+        <is>
+          <t>16/10/2023 22:28</t>
+        </is>
+      </c>
+      <c r="N130" t="n">
+        <v>3.19</v>
+      </c>
+      <c r="O130" t="inlineStr">
+        <is>
+          <t>13/10/2023 06:12</t>
+        </is>
+      </c>
+      <c r="P130" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="Q130" t="inlineStr">
+        <is>
+          <t>16/10/2023 22:28</t>
+        </is>
+      </c>
+      <c r="R130" t="n">
+        <v>2.22</v>
+      </c>
+      <c r="S130" t="inlineStr">
+        <is>
+          <t>13/10/2023 06:12</t>
+        </is>
+      </c>
+      <c r="T130" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="U130" t="inlineStr">
+        <is>
+          <t>16/10/2023 22:28</t>
+        </is>
+      </c>
+      <c r="V130" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/boca-juniors-de-cali-fortaleza-c-e-i-f/pjL44O8D/</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>primera-b</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E131" s="2" t="n">
+        <v>45215.95833333334</v>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>Leones</t>
+        </is>
+      </c>
+      <c r="G131" t="n">
+        <v>2</v>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>Cartagena</t>
+        </is>
+      </c>
+      <c r="I131" t="n">
+        <v>1</v>
+      </c>
+      <c r="J131" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="K131" t="inlineStr">
+        <is>
+          <t>13/10/2023 06:12</t>
+        </is>
+      </c>
+      <c r="L131" t="n">
+        <v>2.16</v>
+      </c>
+      <c r="M131" t="inlineStr">
+        <is>
+          <t>16/10/2023 22:59</t>
+        </is>
+      </c>
+      <c r="N131" t="n">
+        <v>3.51</v>
+      </c>
+      <c r="O131" t="inlineStr">
+        <is>
+          <t>13/10/2023 06:12</t>
+        </is>
+      </c>
+      <c r="P131" t="n">
+        <v>3.42</v>
+      </c>
+      <c r="Q131" t="inlineStr">
+        <is>
+          <t>16/10/2023 22:59</t>
+        </is>
+      </c>
+      <c r="R131" t="n">
+        <v>3.55</v>
+      </c>
+      <c r="S131" t="inlineStr">
+        <is>
+          <t>13/10/2023 06:12</t>
+        </is>
+      </c>
+      <c r="T131" t="n">
+        <v>3.44</v>
+      </c>
+      <c r="U131" t="inlineStr">
+        <is>
+          <t>16/10/2023 22:59</t>
+        </is>
+      </c>
+      <c r="V131" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/leones-cartagena/hfRKAaVn/</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n">
+        <v>131</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>primera-b</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E132" s="2" t="n">
+        <v>45217.9375</v>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>Barranquilla</t>
+        </is>
+      </c>
+      <c r="G132" t="n">
+        <v>2</v>
+      </c>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>Atletico F.C.</t>
+        </is>
+      </c>
+      <c r="I132" t="n">
+        <v>1</v>
+      </c>
+      <c r="J132" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="K132" t="inlineStr">
+        <is>
+          <t>13/10/2023 10:50</t>
+        </is>
+      </c>
+      <c r="L132" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="M132" t="inlineStr">
+        <is>
+          <t>18/10/2023 22:27</t>
+        </is>
+      </c>
+      <c r="N132" t="n">
+        <v>3.27</v>
+      </c>
+      <c r="O132" t="inlineStr">
+        <is>
+          <t>13/10/2023 10:50</t>
+        </is>
+      </c>
+      <c r="P132" t="n">
+        <v>2.95</v>
+      </c>
+      <c r="Q132" t="inlineStr">
+        <is>
+          <t>18/10/2023 22:28</t>
+        </is>
+      </c>
+      <c r="R132" t="n">
+        <v>3.31</v>
+      </c>
+      <c r="S132" t="inlineStr">
+        <is>
+          <t>13/10/2023 10:50</t>
+        </is>
+      </c>
+      <c r="T132" t="n">
+        <v>3.12</v>
+      </c>
+      <c r="U132" t="inlineStr">
+        <is>
+          <t>18/10/2023 22:25</t>
+        </is>
+      </c>
+      <c r="V132" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/barranquilla-atletico-f-c/ETHu6ypI/</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>primera-b</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E133" s="2" t="n">
+        <v>45218.04166666666</v>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>Cucuta</t>
+        </is>
+      </c>
+      <c r="G133" t="n">
+        <v>3</v>
+      </c>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>Llaneros</t>
+        </is>
+      </c>
+      <c r="I133" t="n">
+        <v>2</v>
+      </c>
+      <c r="J133" t="n">
+        <v>2.13</v>
+      </c>
+      <c r="K133" t="inlineStr">
+        <is>
+          <t>13/10/2023 10:50</t>
+        </is>
+      </c>
+      <c r="L133" t="n">
+        <v>2.09</v>
+      </c>
+      <c r="M133" t="inlineStr">
+        <is>
+          <t>19/10/2023 00:31</t>
+        </is>
+      </c>
+      <c r="N133" t="n">
+        <v>2.96</v>
+      </c>
+      <c r="O133" t="inlineStr">
+        <is>
+          <t>13/10/2023 10:50</t>
+        </is>
+      </c>
+      <c r="P133" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="Q133" t="inlineStr">
+        <is>
+          <t>19/10/2023 00:31</t>
+        </is>
+      </c>
+      <c r="R133" t="n">
+        <v>3.86</v>
+      </c>
+      <c r="S133" t="inlineStr">
+        <is>
+          <t>13/10/2023 10:50</t>
+        </is>
+      </c>
+      <c r="T133" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="U133" t="inlineStr">
+        <is>
+          <t>19/10/2023 00:31</t>
+        </is>
+      </c>
+      <c r="V133" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/cucuta-llaneros/Q7obOIan/</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>primera-b</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E134" s="2" t="n">
+        <v>45221.875</v>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>Fortaleza</t>
+        </is>
+      </c>
+      <c r="G134" t="n">
+        <v>2</v>
+      </c>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>Leones</t>
+        </is>
+      </c>
+      <c r="I134" t="n">
+        <v>1</v>
+      </c>
+      <c r="J134" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="K134" t="inlineStr">
+        <is>
+          <t>16/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="L134" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="M134" t="inlineStr">
+        <is>
+          <t>22/10/2023 20:59</t>
+        </is>
+      </c>
+      <c r="N134" t="n">
+        <v>4.12</v>
+      </c>
+      <c r="O134" t="inlineStr">
+        <is>
+          <t>16/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="P134" t="n">
+        <v>4.39</v>
+      </c>
+      <c r="Q134" t="inlineStr">
+        <is>
+          <t>22/10/2023 20:59</t>
+        </is>
+      </c>
+      <c r="R134" t="n">
+        <v>5.43</v>
+      </c>
+      <c r="S134" t="inlineStr">
+        <is>
+          <t>16/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="T134" t="n">
+        <v>6.38</v>
+      </c>
+      <c r="U134" t="inlineStr">
+        <is>
+          <t>22/10/2023 20:59</t>
+        </is>
+      </c>
+      <c r="V134" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/fortaleza-c-e-i-f-leones/GATm869l/</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>primera-b</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E135" s="2" t="n">
+        <v>45222.04166666666</v>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>Cartagena</t>
+        </is>
+      </c>
+      <c r="G135" t="n">
+        <v>1</v>
+      </c>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>Boca Juniors</t>
+        </is>
+      </c>
+      <c r="I135" t="n">
+        <v>0</v>
+      </c>
+      <c r="J135" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="K135" t="inlineStr">
+        <is>
+          <t>16/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="L135" t="n">
+        <v>1.87</v>
+      </c>
+      <c r="M135" t="inlineStr">
+        <is>
+          <t>23/10/2023 00:52</t>
+        </is>
+      </c>
+      <c r="N135" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="O135" t="inlineStr">
+        <is>
+          <t>16/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="P135" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="Q135" t="inlineStr">
+        <is>
+          <t>23/10/2023 00:52</t>
+        </is>
+      </c>
+      <c r="R135" t="n">
+        <v>4.12</v>
+      </c>
+      <c r="S135" t="inlineStr">
+        <is>
+          <t>16/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="T135" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="U135" t="inlineStr">
+        <is>
+          <t>23/10/2023 00:52</t>
+        </is>
+      </c>
+      <c r="V135" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/cartagena-boca-juniors-de-cali/AVyGBuGt/</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>primera-b</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E136" s="2" t="n">
+        <v>45223.02083333334</v>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>Atletico F.C.</t>
+        </is>
+      </c>
+      <c r="G136" t="n">
+        <v>1</v>
+      </c>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>Cucuta</t>
+        </is>
+      </c>
+      <c r="I136" t="n">
+        <v>1</v>
+      </c>
+      <c r="J136" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>19/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="L136" t="n">
+        <v>3.42</v>
+      </c>
+      <c r="M136" t="inlineStr">
+        <is>
+          <t>23/10/2023 22:29</t>
+        </is>
+      </c>
+      <c r="N136" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="O136" t="inlineStr">
+        <is>
+          <t>19/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="P136" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="Q136" t="inlineStr">
+        <is>
+          <t>23/10/2023 22:29</t>
+        </is>
+      </c>
+      <c r="R136" t="n">
+        <v>2.28</v>
+      </c>
+      <c r="S136" t="inlineStr">
+        <is>
+          <t>19/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="T136" t="n">
+        <v>2.31</v>
+      </c>
+      <c r="U136" t="inlineStr">
+        <is>
+          <t>23/10/2023 22:29</t>
+        </is>
+      </c>
+      <c r="V136" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/atletico-f-c-cucuta/neeMIETN/</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>primera-b</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E137" s="2" t="n">
+        <v>45223.10416666666</v>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>Llaneros</t>
+        </is>
+      </c>
+      <c r="G137" t="n">
+        <v>4</v>
+      </c>
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>Barranquilla</t>
+        </is>
+      </c>
+      <c r="I137" t="n">
+        <v>2</v>
+      </c>
+      <c r="J137" t="n">
+        <v>1.52</v>
+      </c>
+      <c r="K137" t="inlineStr">
+        <is>
+          <t>19/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="L137" t="n">
+        <v>1.52</v>
+      </c>
+      <c r="M137" t="inlineStr">
+        <is>
+          <t>24/10/2023 00:07</t>
+        </is>
+      </c>
+      <c r="N137" t="n">
+        <v>4.11</v>
+      </c>
+      <c r="O137" t="inlineStr">
+        <is>
+          <t>19/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="P137" t="n">
+        <v>4.04</v>
+      </c>
+      <c r="Q137" t="inlineStr">
+        <is>
+          <t>24/10/2023 00:07</t>
+        </is>
+      </c>
+      <c r="R137" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="S137" t="inlineStr">
+        <is>
+          <t>19/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="T137" t="n">
+        <v>6.98</v>
+      </c>
+      <c r="U137" t="inlineStr">
+        <is>
+          <t>24/10/2023 00:07</t>
+        </is>
+      </c>
+      <c r="V137" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/llaneros-barranquilla/nsGm4FEU/</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>primera-b</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E138" s="2" t="n">
+        <v>45225.875</v>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>Leones</t>
+        </is>
+      </c>
+      <c r="G138" t="n">
+        <v>3</v>
+      </c>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>Boca Juniors</t>
+        </is>
+      </c>
+      <c r="I138" t="n">
+        <v>2</v>
+      </c>
+      <c r="J138" t="n">
+        <v>1.92</v>
+      </c>
+      <c r="K138" t="inlineStr">
+        <is>
+          <t>23/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="L138" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="M138" t="inlineStr">
+        <is>
+          <t>26/10/2023 20:58</t>
+        </is>
+      </c>
+      <c r="N138" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="O138" t="inlineStr">
+        <is>
+          <t>23/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="P138" t="n">
+        <v>3.88</v>
+      </c>
+      <c r="Q138" t="inlineStr">
+        <is>
+          <t>26/10/2023 20:49</t>
+        </is>
+      </c>
+      <c r="R138" t="n">
+        <v>3.87</v>
+      </c>
+      <c r="S138" t="inlineStr">
+        <is>
+          <t>23/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="T138" t="n">
+        <v>4.25</v>
+      </c>
+      <c r="U138" t="inlineStr">
+        <is>
+          <t>26/10/2023 20:49</t>
+        </is>
+      </c>
+      <c r="V138" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/leones-boca-juniors-de-cali/I1OW7cF5/</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>primera-b</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E139" s="2" t="n">
+        <v>45226.03125</v>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>Cartagena</t>
+        </is>
+      </c>
+      <c r="G139" t="n">
+        <v>1</v>
+      </c>
+      <c r="H139" t="inlineStr">
+        <is>
+          <t>Fortaleza</t>
+        </is>
+      </c>
+      <c r="I139" t="n">
+        <v>2</v>
+      </c>
+      <c r="J139" t="n">
+        <v>2.85</v>
+      </c>
+      <c r="K139" t="inlineStr">
+        <is>
+          <t>23/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="L139" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="M139" t="inlineStr">
+        <is>
+          <t>26/10/2023 23:52</t>
+        </is>
+      </c>
+      <c r="N139" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="O139" t="inlineStr">
+        <is>
+          <t>23/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="P139" t="n">
+        <v>3.09</v>
+      </c>
+      <c r="Q139" t="inlineStr">
+        <is>
+          <t>26/10/2023 23:51</t>
+        </is>
+      </c>
+      <c r="R139" t="n">
+        <v>2.63</v>
+      </c>
+      <c r="S139" t="inlineStr">
+        <is>
+          <t>23/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="T139" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="U139" t="inlineStr">
+        <is>
+          <t>26/10/2023 23:52</t>
+        </is>
+      </c>
+      <c r="V139" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/cartagena-fortaleza-c-e-i-f/lORe6pv1/</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>primera-b</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E140" s="2" t="n">
+        <v>45226.9375</v>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>Atletico F.C.</t>
+        </is>
+      </c>
+      <c r="G140" t="n">
+        <v>2</v>
+      </c>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>Llaneros</t>
+        </is>
+      </c>
+      <c r="I140" t="n">
+        <v>2</v>
+      </c>
+      <c r="J140" t="n">
+        <v>2.83</v>
+      </c>
+      <c r="K140" t="inlineStr">
+        <is>
+          <t>24/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="L140" t="n">
+        <v>3.72</v>
+      </c>
+      <c r="M140" t="inlineStr">
+        <is>
+          <t>27/10/2023 22:21</t>
+        </is>
+      </c>
+      <c r="N140" t="n">
+        <v>3.04</v>
+      </c>
+      <c r="O140" t="inlineStr">
+        <is>
+          <t>24/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="P140" t="n">
+        <v>2.93</v>
+      </c>
+      <c r="Q140" t="inlineStr">
+        <is>
+          <t>27/10/2023 22:28</t>
+        </is>
+      </c>
+      <c r="R140" t="n">
+        <v>2.69</v>
+      </c>
+      <c r="S140" t="inlineStr">
+        <is>
+          <t>24/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="T140" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="U140" t="inlineStr">
+        <is>
+          <t>27/10/2023 22:21</t>
+        </is>
+      </c>
+      <c r="V140" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/atletico-f-c-llaneros/IF35MdUb/</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>primera-b</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E141" s="2" t="n">
+        <v>45226.95833333334</v>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>Barranquilla</t>
+        </is>
+      </c>
+      <c r="G141" t="n">
+        <v>0</v>
+      </c>
+      <c r="H141" t="inlineStr">
+        <is>
+          <t>Cucuta</t>
+        </is>
+      </c>
+      <c r="I141" t="n">
+        <v>1</v>
+      </c>
+      <c r="J141" t="n">
+        <v>3.41</v>
+      </c>
+      <c r="K141" t="inlineStr">
+        <is>
+          <t>24/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="L141" t="n">
+        <v>3.22</v>
+      </c>
+      <c r="M141" t="inlineStr">
+        <is>
+          <t>27/10/2023 22:59</t>
+        </is>
+      </c>
+      <c r="N141" t="n">
+        <v>3.28</v>
+      </c>
+      <c r="O141" t="inlineStr">
+        <is>
+          <t>24/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="P141" t="n">
+        <v>3.38</v>
+      </c>
+      <c r="Q141" t="inlineStr">
+        <is>
+          <t>27/10/2023 22:59</t>
+        </is>
+      </c>
+      <c r="R141" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="S141" t="inlineStr">
+        <is>
+          <t>24/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="T141" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="U141" t="inlineStr">
+        <is>
+          <t>27/10/2023 22:59</t>
+        </is>
+      </c>
+      <c r="V141" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/barranquilla-cucuta/84dIJfEH/</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>primera-b</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E142" s="2" t="n">
+        <v>45229.91666666666</v>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>Cucuta</t>
+        </is>
+      </c>
+      <c r="G142" t="n">
+        <v>1</v>
+      </c>
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>Barranquilla</t>
+        </is>
+      </c>
+      <c r="I142" t="n">
+        <v>0</v>
+      </c>
+      <c r="J142" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="K142" t="inlineStr">
+        <is>
+          <t>27/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="L142" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="M142" t="inlineStr">
+        <is>
+          <t>30/10/2023 21:20</t>
+        </is>
+      </c>
+      <c r="N142" t="n">
+        <v>4.53</v>
+      </c>
+      <c r="O142" t="inlineStr">
+        <is>
+          <t>27/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="P142" t="n">
+        <v>5.04</v>
+      </c>
+      <c r="Q142" t="inlineStr">
+        <is>
+          <t>30/10/2023 21:20</t>
+        </is>
+      </c>
+      <c r="R142" t="n">
+        <v>7.29</v>
+      </c>
+      <c r="S142" t="inlineStr">
+        <is>
+          <t>27/10/2023 23:12</t>
+        </is>
+      </c>
+      <c r="T142" t="n">
+        <v>8.380000000000001</v>
+      </c>
+      <c r="U142" t="inlineStr">
+        <is>
+          <t>30/10/2023 21:20</t>
+        </is>
+      </c>
+      <c r="V142" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/cucuta-barranquilla/0vgALGq5/</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>primera-b</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E143" s="2" t="n">
+        <v>45230.89583333334</v>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>Boca Juniors</t>
+        </is>
+      </c>
+      <c r="G143" t="n">
+        <v>3</v>
+      </c>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>Leones</t>
+        </is>
+      </c>
+      <c r="I143" t="n">
+        <v>3</v>
+      </c>
+      <c r="J143" t="n">
+        <v>2.03</v>
+      </c>
+      <c r="K143" t="inlineStr">
+        <is>
+          <t>26/10/2023 21:12</t>
+        </is>
+      </c>
+      <c r="L143" t="n">
+        <v>3.37</v>
+      </c>
+      <c r="M143" t="inlineStr">
+        <is>
+          <t>31/10/2023 21:29</t>
+        </is>
+      </c>
+      <c r="N143" t="n">
+        <v>3.52</v>
+      </c>
+      <c r="O143" t="inlineStr">
+        <is>
+          <t>26/10/2023 21:12</t>
+        </is>
+      </c>
+      <c r="P143" t="n">
+        <v>3.74</v>
+      </c>
+      <c r="Q143" t="inlineStr">
+        <is>
+          <t>31/10/2023 21:29</t>
+        </is>
+      </c>
+      <c r="R143" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="S143" t="inlineStr">
+        <is>
+          <t>26/10/2023 21:12</t>
+        </is>
+      </c>
+      <c r="T143" t="n">
+        <v>1.93</v>
+      </c>
+      <c r="U143" t="inlineStr">
+        <is>
+          <t>31/10/2023 21:29</t>
+        </is>
+      </c>
+      <c r="V143" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/boca-juniors-de-cali-leones/vBPS8w0a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>primera-b</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E144" s="2" t="n">
+        <v>45230.95833333334</v>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>Fortaleza</t>
+        </is>
+      </c>
+      <c r="G144" t="n">
+        <v>3</v>
+      </c>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>Cartagena</t>
+        </is>
+      </c>
+      <c r="I144" t="n">
+        <v>0</v>
+      </c>
+      <c r="J144" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="K144" t="inlineStr">
+        <is>
+          <t>27/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="L144" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="M144" t="inlineStr">
+        <is>
+          <t>31/10/2023 22:59</t>
+        </is>
+      </c>
+      <c r="N144" t="n">
+        <v>4.01</v>
+      </c>
+      <c r="O144" t="inlineStr">
+        <is>
+          <t>27/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="P144" t="n">
+        <v>4.53</v>
+      </c>
+      <c r="Q144" t="inlineStr">
+        <is>
+          <t>31/10/2023 22:59</t>
+        </is>
+      </c>
+      <c r="R144" t="n">
+        <v>5.87</v>
+      </c>
+      <c r="S144" t="inlineStr">
+        <is>
+          <t>27/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="T144" t="n">
+        <v>10.37</v>
+      </c>
+      <c r="U144" t="inlineStr">
+        <is>
+          <t>31/10/2023 22:59</t>
+        </is>
+      </c>
+      <c r="V144" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/fortaleza-c-e-i-f-cartagena/4zQq9nfr/</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>primera-b</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E145" s="2" t="n">
+        <v>45231.06944444445</v>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>Llaneros</t>
+        </is>
+      </c>
+      <c r="G145" t="n">
+        <v>1</v>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>Atletico F.C.</t>
+        </is>
+      </c>
+      <c r="I145" t="n">
+        <v>0</v>
+      </c>
+      <c r="J145" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="K145" t="inlineStr">
+        <is>
+          <t>27/10/2023 22:42</t>
+        </is>
+      </c>
+      <c r="L145" t="n">
+        <v>1.49</v>
+      </c>
+      <c r="M145" t="inlineStr">
+        <is>
+          <t>01/11/2023 01:31</t>
+        </is>
+      </c>
+      <c r="N145" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="O145" t="inlineStr">
+        <is>
+          <t>27/10/2023 22:42</t>
+        </is>
+      </c>
+      <c r="P145" t="n">
+        <v>3.96</v>
+      </c>
+      <c r="Q145" t="inlineStr">
+        <is>
+          <t>01/11/2023 01:31</t>
+        </is>
+      </c>
+      <c r="R145" t="n">
+        <v>6.24</v>
+      </c>
+      <c r="S145" t="inlineStr">
+        <is>
+          <t>27/10/2023 22:42</t>
+        </is>
+      </c>
+      <c r="T145" t="n">
+        <v>7.86</v>
+      </c>
+      <c r="U145" t="inlineStr">
+        <is>
+          <t>01/11/2023 01:31</t>
+        </is>
+      </c>
+      <c r="V145" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/llaneros-atletico-f-c/nHnfPbpt/</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>primera-b</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E146" s="2" t="n">
+        <v>45234.89583333334</v>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>Boca Juniors</t>
+        </is>
+      </c>
+      <c r="G146" t="n">
+        <v>2</v>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>Cartagena</t>
+        </is>
+      </c>
+      <c r="I146" t="n">
+        <v>1</v>
+      </c>
+      <c r="J146" t="n">
+        <v>2.26</v>
+      </c>
+      <c r="K146" t="inlineStr">
+        <is>
+          <t>01/11/2023 12:43</t>
+        </is>
+      </c>
+      <c r="L146" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="M146" t="inlineStr">
+        <is>
+          <t>04/11/2023 20:33</t>
+        </is>
+      </c>
+      <c r="N146" t="n">
+        <v>3.31</v>
+      </c>
+      <c r="O146" t="inlineStr">
+        <is>
+          <t>01/11/2023 12:43</t>
+        </is>
+      </c>
+      <c r="P146" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="Q146" t="inlineStr">
+        <is>
+          <t>04/11/2023 20:54</t>
+        </is>
+      </c>
+      <c r="R146" t="n">
+        <v>3.23</v>
+      </c>
+      <c r="S146" t="inlineStr">
+        <is>
+          <t>01/11/2023 12:43</t>
+        </is>
+      </c>
+      <c r="T146" t="n">
+        <v>3.38</v>
+      </c>
+      <c r="U146" t="inlineStr">
+        <is>
+          <t>04/11/2023 20:54</t>
+        </is>
+      </c>
+      <c r="V146" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/boca-juniors-de-cali-cartagena/WpQO9Jpg/</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>primera-b</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E147" s="2" t="n">
+        <v>45235.0625</v>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>Leones</t>
+        </is>
+      </c>
+      <c r="G147" t="n">
+        <v>3</v>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>Fortaleza</t>
+        </is>
+      </c>
+      <c r="I147" t="n">
+        <v>0</v>
+      </c>
+      <c r="J147" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="K147" t="inlineStr">
+        <is>
+          <t>01/11/2023 12:43</t>
+        </is>
+      </c>
+      <c r="L147" t="n">
+        <v>2.91</v>
+      </c>
+      <c r="M147" t="inlineStr">
+        <is>
+          <t>05/11/2023 01:26</t>
+        </is>
+      </c>
+      <c r="N147" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="O147" t="inlineStr">
+        <is>
+          <t>01/11/2023 12:43</t>
+        </is>
+      </c>
+      <c r="P147" t="n">
+        <v>3.51</v>
+      </c>
+      <c r="Q147" t="inlineStr">
+        <is>
+          <t>05/11/2023 01:26</t>
+        </is>
+      </c>
+      <c r="R147" t="n">
+        <v>2.43</v>
+      </c>
+      <c r="S147" t="inlineStr">
+        <is>
+          <t>01/11/2023 12:43</t>
+        </is>
+      </c>
+      <c r="T147" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="U147" t="inlineStr">
+        <is>
+          <t>05/11/2023 01:26</t>
+        </is>
+      </c>
+      <c r="V147" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/leones-fortaleza-c-e-i-f/6aM054g7/</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>primera-b</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E148" s="2" t="n">
+        <v>45236.0625</v>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>Barranquilla</t>
+        </is>
+      </c>
+      <c r="G148" t="n">
+        <v>0</v>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>Llaneros</t>
+        </is>
+      </c>
+      <c r="I148" t="n">
+        <v>0</v>
+      </c>
+      <c r="J148" t="n">
+        <v>3.19</v>
+      </c>
+      <c r="K148" t="inlineStr">
+        <is>
+          <t>01/11/2023 12:43</t>
+        </is>
+      </c>
+      <c r="L148" t="n">
+        <v>5.22</v>
+      </c>
+      <c r="M148" t="inlineStr">
+        <is>
+          <t>06/11/2023 01:28</t>
+        </is>
+      </c>
+      <c r="N148" t="n">
+        <v>3.19</v>
+      </c>
+      <c r="O148" t="inlineStr">
+        <is>
+          <t>01/11/2023 12:43</t>
+        </is>
+      </c>
+      <c r="P148" t="n">
+        <v>3.82</v>
+      </c>
+      <c r="Q148" t="inlineStr">
+        <is>
+          <t>06/11/2023 01:28</t>
+        </is>
+      </c>
+      <c r="R148" t="n">
+        <v>2.34</v>
+      </c>
+      <c r="S148" t="inlineStr">
+        <is>
+          <t>01/11/2023 12:43</t>
+        </is>
+      </c>
+      <c r="T148" t="n">
+        <v>1.68</v>
+      </c>
+      <c r="U148" t="inlineStr">
+        <is>
+          <t>06/11/2023 01:28</t>
+        </is>
+      </c>
+      <c r="V148" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/barranquilla-llaneros/KUp2NxFh/</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="n">
+        <v>148</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>primera-b</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E149" s="2" t="n">
+        <v>45238.95833333334</v>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>Cucuta</t>
+        </is>
+      </c>
+      <c r="G149" t="n">
+        <v>1</v>
+      </c>
+      <c r="H149" t="inlineStr">
+        <is>
+          <t>Atletico F.C.</t>
+        </is>
+      </c>
+      <c r="I149" t="n">
+        <v>0</v>
+      </c>
+      <c r="J149" t="n">
+        <v>1.46</v>
+      </c>
+      <c r="K149" t="inlineStr">
+        <is>
+          <t>01/11/2023 22:12</t>
+        </is>
+      </c>
+      <c r="L149" t="n">
+        <v>1.39</v>
+      </c>
+      <c r="M149" t="inlineStr">
+        <is>
+          <t>08/11/2023 22:55</t>
+        </is>
+      </c>
+      <c r="N149" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="O149" t="inlineStr">
+        <is>
+          <t>01/11/2023 22:12</t>
+        </is>
+      </c>
+      <c r="P149" t="n">
+        <v>4.88</v>
+      </c>
+      <c r="Q149" t="inlineStr">
+        <is>
+          <t>08/11/2023 22:57</t>
+        </is>
+      </c>
+      <c r="R149" t="n">
+        <v>6.74</v>
+      </c>
+      <c r="S149" t="inlineStr">
+        <is>
+          <t>01/11/2023 22:12</t>
+        </is>
+      </c>
+      <c r="T149" t="n">
+        <v>7.77</v>
+      </c>
+      <c r="U149" t="inlineStr">
+        <is>
+          <t>08/11/2023 22:57</t>
+        </is>
+      </c>
+      <c r="V149" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/cucuta-atletico-f-c/vViEKzaB/</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>primera-b</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E150" s="2" t="n">
+        <v>45241.91666666666</v>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>Atletico F.C.</t>
+        </is>
+      </c>
+      <c r="G150" t="n">
+        <v>0</v>
+      </c>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>Barranquilla</t>
+        </is>
+      </c>
+      <c r="I150" t="n">
+        <v>0</v>
+      </c>
+      <c r="J150" t="n">
+        <v>1.79</v>
+      </c>
+      <c r="K150" t="inlineStr">
+        <is>
+          <t>08/11/2023 23:13</t>
+        </is>
+      </c>
+      <c r="L150" t="n">
+        <v>1.69</v>
+      </c>
+      <c r="M150" t="inlineStr">
+        <is>
+          <t>11/11/2023 21:59</t>
+        </is>
+      </c>
+      <c r="N150" t="n">
+        <v>3.69</v>
+      </c>
+      <c r="O150" t="inlineStr">
+        <is>
+          <t>08/11/2023 23:13</t>
+        </is>
+      </c>
+      <c r="P150" t="n">
+        <v>3.93</v>
+      </c>
+      <c r="Q150" t="inlineStr">
+        <is>
+          <t>11/11/2023 21:59</t>
+        </is>
+      </c>
+      <c r="R150" t="n">
+        <v>4.37</v>
+      </c>
+      <c r="S150" t="inlineStr">
+        <is>
+          <t>08/11/2023 23:13</t>
+        </is>
+      </c>
+      <c r="T150" t="n">
+        <v>4.93</v>
+      </c>
+      <c r="U150" t="inlineStr">
+        <is>
+          <t>11/11/2023 21:59</t>
+        </is>
+      </c>
+      <c r="V150" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/atletico-f-c-barranquilla/8jHq5eaO/</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>primera-b</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E151" s="2" t="n">
+        <v>45241.91666666666</v>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>Llaneros</t>
+        </is>
+      </c>
+      <c r="G151" t="n">
+        <v>1</v>
+      </c>
+      <c r="H151" t="inlineStr">
+        <is>
+          <t>Cucuta</t>
+        </is>
+      </c>
+      <c r="I151" t="n">
+        <v>0</v>
+      </c>
+      <c r="J151" t="n">
+        <v>2.04</v>
+      </c>
+      <c r="K151" t="inlineStr">
+        <is>
+          <t>08/11/2023 23:13</t>
+        </is>
+      </c>
+      <c r="L151" t="n">
+        <v>1.41</v>
+      </c>
+      <c r="M151" t="inlineStr">
+        <is>
+          <t>11/11/2023 21:57</t>
+        </is>
+      </c>
+      <c r="N151" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="O151" t="inlineStr">
+        <is>
+          <t>08/11/2023 23:13</t>
+        </is>
+      </c>
+      <c r="P151" t="n">
+        <v>4.12</v>
+      </c>
+      <c r="Q151" t="inlineStr">
+        <is>
+          <t>11/11/2023 21:57</t>
+        </is>
+      </c>
+      <c r="R151" t="n">
+        <v>4.01</v>
+      </c>
+      <c r="S151" t="inlineStr">
+        <is>
+          <t>08/11/2023 23:13</t>
+        </is>
+      </c>
+      <c r="T151" t="n">
+        <v>8.76</v>
+      </c>
+      <c r="U151" t="inlineStr">
+        <is>
+          <t>11/11/2023 21:57</t>
+        </is>
+      </c>
+      <c r="V151" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/llaneros-cucuta/0QDy7HUB/</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="1" t="n">
+        <v>151</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>primera-b</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E152" s="2" t="n">
+        <v>45242.01041666666</v>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>Fortaleza</t>
+        </is>
+      </c>
+      <c r="G152" t="n">
+        <v>2</v>
+      </c>
+      <c r="H152" t="inlineStr">
+        <is>
+          <t>Boca Juniors</t>
+        </is>
+      </c>
+      <c r="I152" t="n">
+        <v>1</v>
+      </c>
+      <c r="J152" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="K152" t="inlineStr">
+        <is>
+          <t>08/11/2023 03:42</t>
+        </is>
+      </c>
+      <c r="L152" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="M152" t="inlineStr">
+        <is>
+          <t>12/11/2023 00:11</t>
+        </is>
+      </c>
+      <c r="N152" t="n">
+        <v>4.61</v>
+      </c>
+      <c r="O152" t="inlineStr">
+        <is>
+          <t>08/11/2023 03:42</t>
+        </is>
+      </c>
+      <c r="P152" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="Q152" t="inlineStr">
+        <is>
+          <t>12/11/2023 00:11</t>
+        </is>
+      </c>
+      <c r="R152" t="n">
+        <v>6.88</v>
+      </c>
+      <c r="S152" t="inlineStr">
+        <is>
+          <t>08/11/2023 03:42</t>
+        </is>
+      </c>
+      <c r="T152" t="n">
+        <v>11.93</v>
+      </c>
+      <c r="U152" t="inlineStr">
+        <is>
+          <t>12/11/2023 00:11</t>
+        </is>
+      </c>
+      <c r="V152" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/fortaleza-c-e-i-f-boca-juniors-de-cali/AXSi7QOf/</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="1" t="n">
+        <v>152</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>primera-b</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E153" s="2" t="n">
+        <v>45242.01041666666</v>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>Cartagena</t>
+        </is>
+      </c>
+      <c r="G153" t="n">
+        <v>1</v>
+      </c>
+      <c r="H153" t="inlineStr">
+        <is>
+          <t>Leones</t>
+        </is>
+      </c>
+      <c r="I153" t="n">
+        <v>1</v>
+      </c>
+      <c r="J153" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="K153" t="inlineStr">
+        <is>
+          <t>08/11/2023 03:42</t>
+        </is>
+      </c>
+      <c r="L153" t="n">
+        <v>5.52</v>
+      </c>
+      <c r="M153" t="inlineStr">
+        <is>
+          <t>11/11/2023 23:37</t>
+        </is>
+      </c>
+      <c r="N153" t="n">
+        <v>3.63</v>
+      </c>
+      <c r="O153" t="inlineStr">
+        <is>
+          <t>08/11/2023 03:42</t>
+        </is>
+      </c>
+      <c r="P153" t="n">
+        <v>4.68</v>
+      </c>
+      <c r="Q153" t="inlineStr">
+        <is>
+          <t>11/11/2023 23:37</t>
+        </is>
+      </c>
+      <c r="R153" t="n">
+        <v>3.39</v>
+      </c>
+      <c r="S153" t="inlineStr">
+        <is>
+          <t>08/11/2023 03:42</t>
+        </is>
+      </c>
+      <c r="T153" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="U153" t="inlineStr">
+        <is>
+          <t>11/11/2023 23:37</t>
+        </is>
+      </c>
+      <c r="V153" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/colombia/primera-b/cartagena-leones/bg9nT7oE/</t>
         </is>
       </c>
     </row>

</xml_diff>